<commit_message>
Add image paste capability to chat sidebar - paste screenshots directly into messages
</commit_message>
<xml_diff>
--- a/shared/artifacts/TGIF_2026_Rollout_Tracking_UNIFIED.xlsx
+++ b/shared/artifacts/TGIF_2026_Rollout_Tracking_UNIFIED.xlsx
@@ -18,7 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,15 +60,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="00006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00C6EFCE"/>
+          <bgColor rgb="00C6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="009C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFEB9C"/>
+          <bgColor rgb="00FFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="009C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFC7CE"/>
+          <bgColor rgb="00FFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -428,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,8 +484,9 @@
     <col width="18" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -503,16 +542,1304 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Project Health</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Project Status</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Project Owner</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Primary Contact</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>62644-LAUDERHILL, FL</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1/20/2026</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1/23/2026</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1/24/2026</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>62652-N. MIAMI BEACH, FL</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1/20/2026</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1/23/2026</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1/24/2026</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>62672-W. MIAMI, FL</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1/20/2026</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1/23/2026</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1/24/2026</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>62486-ATL AIRPORT ATRIUM, GA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1/21/2026</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1/23/2026</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1/24/2026</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45683</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>62037-ATLANTA AIRPORT, GA</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1/21/2026</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1/23/2026</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>1/24/2026</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45683</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>62038-ATLANTA AIRPORT, GA</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1/21/2026</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1/23/2026</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1/24/2026</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45683</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>61755-ATLANTA INTL AIRPORT, GA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1/27/2026</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1/30/2026</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1/31/2026</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>62112-CAMP CREEK, GA</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1/27/2026</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1/30/2026</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1/31/2026</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>62473-LITHONIA, GA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1/27/2026</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1/30/2026</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1/31/2026</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>62115-MALL OF GA, GA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1/28/2026</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>1/30/2026</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1/31/2026</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>62443-SOUTHLAKE, GA</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1/28/2026</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1/30/2026</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1/31/2026</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>61750-GREENBELT, MD</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1/28/2026</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1/30/2026</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1/31/2026</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>62151-LARGO, MD</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2/3/2026</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2/6/2026</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2/7/2026</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45690</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>62149-S. BAL. MORE, MD</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2/3/2026</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2/6/2026</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2/7/2026</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45690</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>62036-SALT SPRING, MD</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2/3/2026</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2/6/2026</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2/7/2026</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45690</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>61742-CHARLOTTE/UNIVERSITY, NC</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2/4/2026</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2/6/2026</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2/7/2026</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45695</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>62641-AVIATION</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2/4/2026</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2/6/2026</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2/7/2026</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45695</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>62508-CHARLOTTE/NORTH LAKE</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2/4/2026</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2/6/2026</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2/7/2026</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45695</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>62643-PEMBROKE PINES</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2/10/2026</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2/13/2026</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2/14/2026</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>On Track</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="K2:K1000">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>"On Track"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>"Some Risk"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>"At Risk"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select from the list" type="list">
+      <formula1>"On Track,Some Risk,At Risk"</formula1>
+    </dataValidation>
+    <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select from the list" type="list">
+      <formula1>"Planning,Configuration,Training,Live,On Hold"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -523,7 +1850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,6 +1904,738 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>62644-LAUDERHILL, FL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>62652-N. MIAMI BEACH, FL</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>62672-W. MIAMI, FL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>62486-ATL AIRPORT ATRIUM, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>62037-ATLANTA AIRPORT, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>62038-ATLANTA AIRPORT, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>61755-ATLANTA INTL AIRPORT, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>62112-CAMP CREEK, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>62473-LITHONIA, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>62115-MALL OF GA, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>62443-SOUTHLAKE, GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>61750-GREENBELT, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>62151-LARGO, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>62149-S. BAL. MORE, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>62036-SALT SPRING, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>61742-CHARLOTTE/UNIVERSITY, NC</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>62641-AVIATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>62508-CHARLOTTE/NORTH LAKE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>62643-PEMBROKE PINES</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bridgeport Restaurant Group, LLC</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>61933-SANDUSKY CEDAR POINT, OH</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>64214 - SOUTH GATE, CA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>64215 - SOUTH GATE, CA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>64216 - NORTH ORANGE, CA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>62633-ORLANDO AIRPORT, FL</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>62668-CHICAGO ERIE STREET, IL</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>62698-EVANSVILLE, IN</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>64206 - ANNAPOLIS, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>64207 - FREDERICK, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>64302 - OWINGS MILLS, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>64303 - ANNE ARUNDEL, MD</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>62703-DETROIT/SOUTHFIELD, MI</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>62693-BLOOMINGTON, MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>62692-MAPLE GROVE, MN</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>64304 - WALDORF, MO</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>64210 - BURLINGTON TOWNSHIP, NJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>64211 - EAST WINDSOR, NJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>64212 - WEST ORANGE, NJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>64213 - LINDEN, NJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>64203 - HYATTSVILLE, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>64208 - GETTYSBURG, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>64209 - BENSALEM, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>64201 - HERNDON, VA</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>64202 - TYSONS CORNER #2 - MCLEAN, VA</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>64205 - WINCHESTER, VA</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>64204 - FRONT ROYAL, WA</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Mera</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>64305-DALLAS/DFW AIRPORT A-12, TX</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Mera</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>64307-DALLAS/DFW AIRPORT B-10, TX</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Mera</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>64308-DALLAS/DFW AIRPORT D-30, TX</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Mera</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>64306-DALLAS/DFW AIRPORTE-17, TX</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Mera</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>64309-FAB.DALLAS/DFW AIRPORT C-30, TX</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>61682-MANAHAWKIN, NJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>61408-TURNERSVILLE, NJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>61091-BETH CHEN, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>61425-DICKSON CITY, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>61684-QUAKERTOWN, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>61680-WILKES BARRE, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>61679-WILLIAMSPORT, PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>RLJ Development</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>61856-BEDFORD PARK, IL</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>United Restaurant Group</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>61520-NEW CASTLE, DE</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>United Restaurant Group</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>62175-DARNEN, NC</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Village 76</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>61896-EFFINGHAM, IL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -588,7 +2647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,6 +2695,110 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Atlanta Restaurant Partners, LLC [Jackmont]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bridgeport Restaurant Group, LLC</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Maui 1 Enterprises, LLC</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mera</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Metz Culinary Management</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RLJ Development</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>United Restaurant Group</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Village 76</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Link Franchise Rollout Playbook Open Sheet button to Dropbox document
</commit_message>
<xml_diff>
--- a/shared/artifacts/TGIF_2026_Rollout_Tracking_UNIFIED.xlsx
+++ b/shared/artifacts/TGIF_2026_Rollout_Tracking_UNIFIED.xlsx
@@ -18,8 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,17 +61,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="00006100"/>
@@ -101,6 +103,17 @@
         <patternFill patternType="solid">
           <fgColor rgb="00FFC7CE"/>
           <bgColor rgb="00FFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="001F4E78"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00DDEBF7"/>
+          <bgColor rgb="00DDEBF7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -466,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +500,16 @@
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
     <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="18" customWidth="1" min="15" max="15"/>
+    <col width="18" customWidth="1" min="16" max="16"/>
+    <col width="18" customWidth="1" min="17" max="17"/>
+    <col width="18" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="21" max="21"/>
+    <col width="18" customWidth="1" min="22" max="22"/>
+    <col width="20" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -557,10 +580,60 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Install Type</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Remote Install Date</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Onsite Install Date</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Remote Training Date</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Onsite Training Date</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Manager Training Date</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Hardware Order #</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Hardware Status</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Hardware Tracking #</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Hardware Delivery Date</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
           <t>Primary Contact</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
@@ -573,8 +646,10 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>45677</v>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>20/01/25</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -627,6 +702,16 @@
         </is>
       </c>
       <c r="N2" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -639,8 +724,10 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>45678</v>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>21/01/25</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -693,6 +780,16 @@
         </is>
       </c>
       <c r="N3" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -705,8 +802,10 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>45678</v>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>21/01/25</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -759,6 +858,16 @@
         </is>
       </c>
       <c r="N4" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -771,8 +880,10 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>45678</v>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>21/01/25</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -825,6 +936,16 @@
         </is>
       </c>
       <c r="N5" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -837,8 +958,10 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>45683</v>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>26/01/25</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -891,6 +1014,16 @@
         </is>
       </c>
       <c r="N6" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -903,8 +1036,10 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>45683</v>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>26/01/25</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -957,6 +1092,16 @@
         </is>
       </c>
       <c r="N7" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -969,8 +1114,10 @@
       <c r="B8" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>45683</v>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>26/01/25</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1023,6 +1170,16 @@
         </is>
       </c>
       <c r="N8" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1035,8 +1192,10 @@
       <c r="B9" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>45684</v>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>27/01/25</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1089,6 +1248,16 @@
         </is>
       </c>
       <c r="N9" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1101,8 +1270,10 @@
       <c r="B10" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>45684</v>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>27/01/25</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1155,6 +1326,16 @@
         </is>
       </c>
       <c r="N10" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1167,8 +1348,10 @@
       <c r="B11" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>45684</v>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>27/01/25</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1221,6 +1404,16 @@
         </is>
       </c>
       <c r="N11" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1233,8 +1426,10 @@
       <c r="B12" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>45689</v>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>01/02/25</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1287,6 +1482,16 @@
         </is>
       </c>
       <c r="N12" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1299,8 +1504,10 @@
       <c r="B13" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>45689</v>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>01/02/25</t>
+        </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1353,6 +1560,16 @@
         </is>
       </c>
       <c r="N13" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1365,8 +1582,10 @@
       <c r="B14" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>45689</v>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>01/02/25</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1419,6 +1638,16 @@
         </is>
       </c>
       <c r="N14" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1431,8 +1660,10 @@
       <c r="B15" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>45690</v>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>02/02/25</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1485,6 +1716,16 @@
         </is>
       </c>
       <c r="N15" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1497,8 +1738,10 @@
       <c r="B16" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>45690</v>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>02/02/25</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1551,6 +1794,16 @@
         </is>
       </c>
       <c r="N16" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1563,8 +1816,10 @@
       <c r="B17" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>45690</v>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>02/02/25</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1617,6 +1872,16 @@
         </is>
       </c>
       <c r="N17" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1629,8 +1894,10 @@
       <c r="B18" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>45695</v>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>07/02/25</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1683,6 +1950,16 @@
         </is>
       </c>
       <c r="N18" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1695,8 +1972,10 @@
       <c r="B19" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>45695</v>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>07/02/25</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1749,6 +2028,16 @@
         </is>
       </c>
       <c r="N19" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1761,8 +2050,10 @@
       <c r="B20" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>45695</v>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>07/02/25</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1815,6 +2106,16 @@
         </is>
       </c>
       <c r="N20" t="inlineStr">
+        <is>
+          <t>Onsite</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>Not Ordered</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1832,12 +2133,32 @@
       <formula>"At Risk"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select from the list" type="list">
+  <conditionalFormatting sqref="U2:U1000">
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="2">
+      <formula>"Not Ordered"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="1">
+      <formula>"Ordered"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3">
+      <formula>"Shipped"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="0">
+      <formula>"Delivered"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Entry" error="Please select from the list" type="list">
       <formula1>"On Track,Some Risk,At Risk"</formula1>
     </dataValidation>
-    <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select from the list" type="list">
+    <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Entry" error="Please select from the list" type="list">
       <formula1>"Planning,Configuration,Training,Live,On Hold"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Entry" error="Please select from the list" type="list">
+      <formula1>"Onsite,Remote,Self Install"</formula1>
+    </dataValidation>
+    <dataValidation sqref="U2:U1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Entry" error="Please select from the list" type="list">
+      <formula1>"Not Ordered,Ordered,Shipped,Delivered"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>